<commit_message>
Working hand for player1
Description of all event handlers till phase 3-1-1
Deletion of an unused handler
Creation of empty fellowship managers
Declaration of player and enemy on a turn
Creation of debug messages
Definition of the four havens
Preparation of the basic hand of player1
Quick fixes on loading order
Other fixes
</commit_message>
<xml_diff>
--- a/developement/stam propiedades cartas.xlsx
+++ b/developement/stam propiedades cartas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Documents\GitHub\erus-will\developement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6DC7B7-51BD-49E6-AE37-7C7DDC37891D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E3499F-2B5A-4DCD-973E-00B54EA0D0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{13B097E6-3838-47CF-AB00-2CC3181D455C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="84">
   <si>
     <t>CLASE</t>
   </si>
@@ -201,18 +201,12 @@
     <t>EVENTO/ACCION</t>
   </si>
   <si>
-    <t>A-fellowship-move</t>
-  </si>
-  <si>
     <t>E-cure</t>
   </si>
   <si>
     <t>E-card-untap</t>
   </si>
   <si>
-    <t>A-location-organize</t>
-  </si>
-  <si>
     <t>E-r-long-event-discard</t>
   </si>
   <si>
@@ -237,58 +231,10 @@
     <t>E-a-long-event-discard</t>
   </si>
   <si>
-    <t>E-move-fellowship</t>
-  </si>
-  <si>
-    <t>P-3-1-0</t>
-  </si>
-  <si>
     <t>P-3-1-1</t>
   </si>
   <si>
     <t>influence</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TAPPED </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UNTAPPED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> WOUNDED</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TAPPED </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UNTAPPED</t>
-    </r>
   </si>
   <si>
     <r>
@@ -323,9 +269,6 @@
     </r>
   </si>
   <si>
-    <t>(draft) DECK</t>
-  </si>
-  <si>
     <t>A-item-store</t>
   </si>
   <si>
@@ -336,13 +279,142 @@
   </si>
   <si>
     <t>(supuesto) ADVERSITY</t>
+  </si>
+  <si>
+    <t>standard-events</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DRAW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HAND MP DISCARD UNTAPPED TAPPED WOUNDED</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DRAW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HAND MP DISCARD UNTAPPED TAPPED</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DRAW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HAND MP DISCARD TAPPED UNTAPPED WOUNDED</t>
+    </r>
+  </si>
+  <si>
+    <t>A-loc-organize</t>
+  </si>
+  <si>
+    <t>A-fell-decl-move</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">entero </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FALSE</t>
+    </r>
+  </si>
+  <si>
+    <t>P-1-1-1 handG</t>
+  </si>
+  <si>
+    <t>CREADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +450,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -510,17 +589,45 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -541,134 +648,6 @@
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -991,15 +970,15 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1028,7 +1007,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1022,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1060,7 +1039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1056,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1073,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1090,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1128,7 +1107,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +1124,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1162,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1156,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1192,7 +1171,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1209,7 +1188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1226,7 +1205,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1243,139 +1222,139 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="D16" s="4"/>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="D17" s="4"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="D18" s="4"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="D19" s="4"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="D20" s="4"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="D21" s="4"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="D22" s="4"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="D23" s="4"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="D24" s="4"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="D25" s="4"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
     </row>
   </sheetData>
@@ -1389,26 +1368,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022EC33C-E900-4004-A9F6-8A74AFDC4BC0}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1428,451 +1408,503 @@
         <v>40</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I2" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I5" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
       <c r="D19" s="4"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
       <c r="D20" s="4"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
       <c r="D21" s="4"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="12"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D22">
@@ -1883,27 +1915,35 @@
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A2:D22">
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="*TODO*">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="*TODO*">
       <formula>NOT(ISERROR(SEARCH("*TODO*",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22 H9:H12 I12">
-    <cfRule type="beginsWith" dxfId="9" priority="5" operator="beginsWith" text="E-">
+  <conditionalFormatting sqref="C2:C22">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="cuantitativo">
+      <formula>NOT(ISERROR(SEARCH("cuantitativo",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="identificativo">
+      <formula>NOT(ISERROR(SEARCH("identificativo",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="estado">
+      <formula>NOT(ISERROR(SEARCH("estado",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G22 H9:H12 J5:J11">
+    <cfRule type="beginsWith" dxfId="3" priority="6" operator="beginsWith" text="A-">
+      <formula>LEFT(G2,LEN("A-"))="A-"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="7" operator="beginsWith" text="E-">
       <formula>LEFT(G2,LEN("E-"))="E-"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="4" operator="beginsWith" text="A-">
-      <formula>LEFT(G2,LEN("A-"))="A-"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I11">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="A-">
+      <formula>LEFT(I5,LEN("A-"))="A-"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C22">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="estado">
-      <formula>NOT(ISERROR(SEARCH("estado",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="identificativo">
-      <formula>NOT(ISERROR(SEARCH("identificativo",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="cuantitativo">
-      <formula>NOT(ISERROR(SEARCH("cuantitativo",C2)))</formula>
+    <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="E-">
+      <formula>LEFT(I5,LEN("E-"))="E-"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Last step before more class specification
Rules for deleting "in" facts after the concerning card has exited the game
Specification of a breadth conflict resolution strategy to reproduce a time-like effect on event-handling sequences
Separation of handG into description and functions
Other fixes
</commit_message>
<xml_diff>
--- a/developement/stam propiedades cartas.xlsx
+++ b/developement/stam propiedades cartas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Documents\GitHub\erus-will\developement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15562AAD-D767-4B8A-94FE-40775D0F2B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80A65C6-7BF8-4308-9D7A-42F832DC738A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{13B097E6-3838-47CF-AB00-2CC3181D455C}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>Pablo Ortega</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{B7024B6A-8036-4E57-82ED-B60C5EEE3C74}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{B7024B6A-8036-4E57-82ED-B60C5EEE3C74}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
   <si>
     <t>CLASE</t>
   </si>
@@ -443,12 +443,24 @@
   <si>
     <t>DEFINIDO</t>
   </si>
+  <si>
+    <t>Leyenda: hay nombres tanto de clases como de interfaces, el tipo de la propiedad indica si puede ser accedido directamente (identificativo o estado) o solo mediante handlers (cuantitativo). *TODO* implica que no se han delimitado todavía los valores o tipos. Los tipos en minúscula hablan son tipos definidos por CLIPS, los que están en mayúscula y son más de uno refieren a un símbolo constante entre ellos, cuando es mayúscula pero es una sola se refiere a una clase no especificada nativamente por CLIPS. El valor en negrita indica su valor predefinido, en ausencia se supone (?default NONE)</t>
+  </si>
+  <si>
+    <t>Leyenda: Nombre en verde para eventos y en amarillo para acciones. Manejado en verde para handler testeado y en naranja para handler incompleto.</t>
+  </si>
+  <si>
+    <t>handG</t>
+  </si>
+  <si>
+    <t>A-item-play</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,13 +496,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -633,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -649,12 +654,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,94 +1296,94 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="D16" s="4"/>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="D17" s="4"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="D18" s="4"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="D19" s="4"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="D20" s="4"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="D21" s="4"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="D22" s="4"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="D23" s="4"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="D24" s="4"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="D25" s="4"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -1428,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022EC33C-E900-4004-A9F6-8A74AFDC4BC0}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,329 +1455,186 @@
     <col min="6" max="6" width="8.26953125" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M10" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" t="s">
-        <v>72</v>
-      </c>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" t="s">
-        <v>72</v>
-      </c>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="I11" t="s">
         <v>72</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="13" t="s">
         <v>72</v>
       </c>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -1774,31 +1642,53 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -1806,132 +1696,358 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" t="s">
+        <v>72</v>
+      </c>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" t="s">
+        <v>72</v>
+      </c>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" t="s">
+        <v>72</v>
+      </c>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="G19" s="3"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="G20" s="3"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="G21" s="3"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="12"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="8"/>
+      <c r="G27" s="3"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="12"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D18">
-    <sortCondition ref="B2:B18"/>
-    <sortCondition ref="A2:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:D27">
+    <sortCondition ref="B11:B27"/>
+    <sortCondition ref="A11:A27"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D6"/>
+    <mergeCell ref="G1:M6"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="A2:D22">
+  <conditionalFormatting sqref="A11:D31">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="*TODO*">
-      <formula>NOT(ISERROR(SEARCH("*TODO*",A2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("*TODO*",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C22">
+  <conditionalFormatting sqref="C11:C31">
     <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="cuantitativo">
-      <formula>NOT(ISERROR(SEARCH("cuantitativo",C2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("cuantitativo",C11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="identificativo">
-      <formula>NOT(ISERROR(SEARCH("identificativo",C2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("identificativo",C11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="estado">
-      <formula>NOT(ISERROR(SEARCH("estado",C2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("estado",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22 H9:H12">
+  <conditionalFormatting sqref="G11:G31 H18:H21">
     <cfRule type="beginsWith" dxfId="3" priority="6" operator="beginsWith" text="A-">
-      <formula>LEFT(G2,LEN("A-"))="A-"</formula>
+      <formula>LEFT(G11,LEN("A-"))="A-"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="7" operator="beginsWith" text="E-">
-      <formula>LEFT(G2,LEN("E-"))="E-"</formula>
+      <formula>LEFT(G11,LEN("E-"))="E-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:J11">
+  <conditionalFormatting sqref="I14 I15:J21">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="A-">
-      <formula>LEFT(I5,LEN("A-"))="A-"</formula>
+      <formula>LEFT(I14,LEN("A-"))="A-"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="E-">
-      <formula>LEFT(I5,LEN("E-"))="E-"</formula>
+      <formula>LEFT(I14,LEN("E-"))="E-"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>